<commit_message>
800 population, 700 polygons and 2000 generations new Test
</commit_message>
<xml_diff>
--- a/kashefi/Test Results.xlsx
+++ b/kashefi/Test Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\University\Genetic Algorithms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\aif-project\kashefi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t>#</t>
   </si>
@@ -77,9 +77,6 @@
     <t>3392.84s</t>
   </si>
   <si>
-    <t>Regular Polygon</t>
-  </si>
-  <si>
     <t>2675.77s</t>
   </si>
   <si>
@@ -135,6 +132,21 @@
   </si>
   <si>
     <t>6252.17s</t>
+  </si>
+  <si>
+    <t>HOF</t>
+  </si>
+  <si>
+    <t>Regular Polygon (5)</t>
+  </si>
+  <si>
+    <t>Regular Polygon (6)</t>
+  </si>
+  <si>
+    <t>31841.32s</t>
+  </si>
+  <si>
+    <t>35567.84s</t>
   </si>
 </sst>
 </file>
@@ -452,30 +464,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M137"/>
+  <dimension ref="A1:N137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="101" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N9"/>
+      <selection activeCell="B12" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,22 +514,25 @@
         <v>13</v>
       </c>
       <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -527,13 +543,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G2">
         <v>300</v>
@@ -542,22 +558,25 @@
         <v>250</v>
       </c>
       <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
         <v>2000</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>3349.08889952153</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.63197531644999705</v>
       </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -568,13 +587,13 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>300</v>
@@ -583,22 +602,25 @@
         <v>250</v>
       </c>
       <c r="I3">
+        <v>20</v>
+      </c>
+      <c r="J3">
         <v>2000</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>3182.3150558213702</v>
       </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3">
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3">
         <v>0.668940741874127</v>
       </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -609,13 +631,13 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G4">
         <v>300</v>
@@ -624,22 +646,25 @@
         <v>250</v>
       </c>
       <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="J4">
         <v>2000</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3197.2309090908998</v>
       </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4">
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4">
         <v>0.67116047041440097</v>
       </c>
-      <c r="M4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -650,13 +675,13 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G5">
         <v>300</v>
@@ -665,22 +690,25 @@
         <v>250</v>
       </c>
       <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
         <v>2000</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>3456.5353110047799</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>11</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.66906025049501505</v>
       </c>
-      <c r="M5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -688,16 +716,16 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G6">
         <v>300</v>
@@ -706,22 +734,25 @@
         <v>250</v>
       </c>
       <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6">
         <v>2000</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>7124.2652950558204</v>
       </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6">
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6">
         <v>0.78407110847528505</v>
       </c>
-      <c r="M6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -729,16 +760,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G7">
         <v>300</v>
@@ -747,22 +778,25 @@
         <v>250</v>
       </c>
       <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="J7">
         <v>2000</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>6307.7538118022303</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>14</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.75283585312892798</v>
       </c>
-      <c r="M7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -770,16 +804,16 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G8">
         <v>300</v>
@@ -788,22 +822,25 @@
         <v>250</v>
       </c>
       <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
         <v>2000</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>5326.22816586921</v>
       </c>
-      <c r="K8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8">
+      <c r="L8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8">
         <v>0.76721929473225003</v>
       </c>
-      <c r="M8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -811,16 +848,16 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G9">
         <v>300</v>
@@ -829,52 +866,94 @@
         <v>250</v>
       </c>
       <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="J9">
         <v>2000</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>6907.31547049441</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>15</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>0.774590842639583</v>
       </c>
-      <c r="M9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10">
+        <v>800</v>
+      </c>
+      <c r="H10">
+        <v>700</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>2000</v>
+      </c>
+      <c r="K10">
+        <v>1533.71795852269</v>
+      </c>
+      <c r="L10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10">
+        <v>0.59226276708125103</v>
+      </c>
+      <c r="N10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>